<commit_message>
draw(layout): add timetable, attendance
</commit_message>
<xml_diff>
--- a/doc/Quản lý sinh viên DB.xlsx
+++ b/doc/Quản lý sinh viên DB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duyho\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Project\23\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BCBF42-D78C-4C07-AA37-AA3D023E8544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C75ABD3-3DB0-4C88-9261-47CAC23602AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>teachers</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>teacher_details</t>
+  </si>
+  <si>
+    <t>courses</t>
+  </si>
+  <si>
+    <t>weekday</t>
   </si>
 </sst>
 </file>
@@ -169,7 +175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +194,12 @@
         <bgColor rgb="FFFBBC04"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,11 +213,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,14 +439,15 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -653,9 +667,7 @@
       <c r="C17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -688,6 +700,9 @@
       <c r="C21" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="I21" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -696,6 +711,9 @@
       <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -704,6 +722,9 @@
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="I23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
@@ -711,6 +732,9 @@
       </c>
       <c r="C24" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>